<commit_message>
new field name for veh
</commit_message>
<xml_diff>
--- a/test/testdata.xlsx
+++ b/test/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vertices" sheetId="1" state="visible" r:id="rId2"/>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">varct Rp</t>
   </si>
   <si>
-    <t xml:space="preserve">varq</t>
+    <t xml:space="preserve">fd</t>
   </si>
   <si>
     <t xml:space="preserve">vardq Rp</t>
@@ -235,19 +235,19 @@
     <t xml:space="preserve">vardct Rp</t>
   </si>
   <si>
-    <t xml:space="preserve">vardq</t>
+    <t xml:space="preserve">vl</t>
   </si>
   <si>
     <t xml:space="preserve">vard Rp</t>
   </si>
   <si>
-    <t xml:space="preserve">vard</t>
+    <t xml:space="preserve">vx</t>
   </si>
   <si>
     <t xml:space="preserve">fix Rp</t>
   </si>
   <si>
-    <t xml:space="preserve">fix</t>
+    <t xml:space="preserve">fp</t>
   </si>
   <si>
     <t xml:space="preserve">KA Siantar Express</t>
@@ -1021,14 +1021,14 @@
     <tableColumn id="9" name="Q"/>
     <tableColumn id="10" name="varq Rp"/>
     <tableColumn id="11" name="varct Rp"/>
-    <tableColumn id="12" name="varq"/>
+    <tableColumn id="12" name="fd"/>
     <tableColumn id="13" name="vardq Rp"/>
     <tableColumn id="14" name="vardct Rp"/>
-    <tableColumn id="15" name="vardq"/>
+    <tableColumn id="15" name="vl"/>
     <tableColumn id="16" name="vard Rp"/>
-    <tableColumn id="17" name="vard"/>
+    <tableColumn id="17" name="vx"/>
     <tableColumn id="18" name="fix Rp"/>
-    <tableColumn id="19" name="fix"/>
+    <tableColumn id="19" name="fp"/>
   </tableColumns>
 </table>
 </file>
@@ -1073,11 +1073,11 @@
   </sheetPr>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.42"/>
@@ -2849,17 +2849,17 @@
   </sheetPr>
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="61.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="61.31"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.01"/>
@@ -8503,7 +8503,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8546,7 +8546,7 @@
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.13"/>

</xml_diff>